<commit_message>
Binary Search Tree (BST)/
</commit_message>
<xml_diff>
--- a/FINAL500.xlsx
+++ b/FINAL500.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code Blocks\Online\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4FDB24-4A14-4101-AA9C-A1640A4BA47F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D288DB64-F6AA-4D81-8EB2-FB4796A3FAE6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="577">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1690,6 +1690,72 @@
   </si>
   <si>
     <t>https://ide.codingblocks.com/s/407406</t>
+  </si>
+  <si>
+    <t>https://ide.codingblocks.com/s/408353</t>
+  </si>
+  <si>
+    <t>https://ide.codingblocks.com/s/408372</t>
+  </si>
+  <si>
+    <t>https://ide.codingblocks.com/s/409079</t>
+  </si>
+  <si>
+    <t>https://ide.codingblocks.com/s/409084</t>
+  </si>
+  <si>
+    <t>https://ide.codingblocks.com/s/409129</t>
+  </si>
+  <si>
+    <t>https://ide.codingblocks.com/s/409988</t>
+  </si>
+  <si>
+    <t>https://ide.codingblocks.com/s/410043</t>
+  </si>
+  <si>
+    <t>Fast Diameter Important</t>
+  </si>
+  <si>
+    <t>https://ide.codingblocks.com/s/411458</t>
+  </si>
+  <si>
+    <t>https://ide.codingblocks.com/s/411463</t>
+  </si>
+  <si>
+    <t>https://ide.codingblocks.com/s/411465</t>
+  </si>
+  <si>
+    <t>https://ide.codingblocks.com/s/411466</t>
+  </si>
+  <si>
+    <t>https://ide.codingblocks.com/s/411625</t>
+  </si>
+  <si>
+    <t>https://ide.codingblocks.com/s/411629</t>
+  </si>
+  <si>
+    <t>https://ide.codingblocks.com/s/412656</t>
+  </si>
+  <si>
+    <t>https://ide.codingblocks.com/s/412757</t>
+  </si>
+  <si>
+    <t>If there are multiple test cases, then remember to make preorder index = 0</t>
+  </si>
+  <si>
+    <t>https://ide.codingblocks.com/s/413068</t>
+  </si>
+  <si>
+    <t>https://ide.codingblocks.com/s/413188</t>
+  </si>
+  <si>
+    <t>https://ide.codingblocks.com/s/413795</t>
+  </si>
+  <si>
+    <t>https://ide.codingblocks.com/s/413832</t>
+  </si>
+  <si>
+    <t>Method-2 Important</t>
   </si>
 </sst>
 </file>
@@ -2121,8 +2187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:E481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A311" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B330" sqref="B330"/>
+    <sheetView tabSelected="1" topLeftCell="A186" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E198" sqref="E198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -3392,7 +3458,10 @@
         <v>107</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
+      </c>
+      <c r="D110" s="10" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="21">
@@ -3403,7 +3472,13 @@
         <v>108</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
+      </c>
+      <c r="D111" s="10" t="s">
+        <v>556</v>
+      </c>
+      <c r="E111" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="21">
@@ -4126,9 +4201,14 @@
         <v>167</v>
       </c>
       <c r="C171" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D171" s="10"/>
+        <v>464</v>
+      </c>
+      <c r="D171" s="10" t="s">
+        <v>560</v>
+      </c>
+      <c r="E171" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="172" spans="1:5" ht="21">
       <c r="A172" s="8" t="s">
@@ -4173,7 +4253,7 @@
       <c r="B176" s="7"/>
       <c r="C176" s="4"/>
     </row>
-    <row r="177" spans="1:3" ht="21">
+    <row r="177" spans="1:5" ht="21">
       <c r="A177" s="5" t="s">
         <v>171</v>
       </c>
@@ -4181,10 +4261,13 @@
         <v>172</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" ht="21">
+        <v>464</v>
+      </c>
+      <c r="D177" s="10" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" ht="21">
       <c r="A178" s="5" t="s">
         <v>171</v>
       </c>
@@ -4192,10 +4275,13 @@
         <v>173</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" ht="21">
+        <v>464</v>
+      </c>
+      <c r="D178" s="10" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" ht="21">
       <c r="A179" s="5" t="s">
         <v>171</v>
       </c>
@@ -4203,10 +4289,13 @@
         <v>174</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" ht="21">
+        <v>464</v>
+      </c>
+      <c r="D179" s="10" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" ht="21">
       <c r="A180" s="5" t="s">
         <v>171</v>
       </c>
@@ -4214,10 +4303,16 @@
         <v>175</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" ht="21">
+        <v>464</v>
+      </c>
+      <c r="D180" s="10" t="s">
+        <v>561</v>
+      </c>
+      <c r="E180" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" ht="21">
       <c r="A181" s="5" t="s">
         <v>171</v>
       </c>
@@ -4228,7 +4323,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="21">
+    <row r="182" spans="1:5" ht="21">
       <c r="A182" s="5" t="s">
         <v>171</v>
       </c>
@@ -4239,7 +4334,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="21">
+    <row r="183" spans="1:5" ht="21">
       <c r="A183" s="5" t="s">
         <v>171</v>
       </c>
@@ -4250,7 +4345,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="184" spans="1:3" ht="21">
+    <row r="184" spans="1:5" ht="21">
       <c r="A184" s="5" t="s">
         <v>171</v>
       </c>
@@ -4261,7 +4356,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="185" spans="1:3" ht="21">
+    <row r="185" spans="1:5" ht="21">
       <c r="A185" s="5" t="s">
         <v>171</v>
       </c>
@@ -4269,10 +4364,13 @@
         <v>180</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" ht="21">
+        <v>464</v>
+      </c>
+      <c r="D185" s="10" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" ht="21">
       <c r="A186" s="5" t="s">
         <v>171</v>
       </c>
@@ -4280,10 +4378,13 @@
         <v>181</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" ht="21">
+        <v>464</v>
+      </c>
+      <c r="D186" s="10" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" ht="21">
       <c r="A187" s="5" t="s">
         <v>171</v>
       </c>
@@ -4291,10 +4392,16 @@
         <v>182</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" ht="21">
+        <v>464</v>
+      </c>
+      <c r="D187" s="10" t="s">
+        <v>565</v>
+      </c>
+      <c r="E187" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" ht="21">
       <c r="A188" s="5" t="s">
         <v>171</v>
       </c>
@@ -4302,10 +4409,16 @@
         <v>183</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" ht="21">
+        <v>464</v>
+      </c>
+      <c r="D188" s="10" t="s">
+        <v>566</v>
+      </c>
+      <c r="E188" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" ht="21">
       <c r="A189" s="5" t="s">
         <v>171</v>
       </c>
@@ -4316,7 +4429,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="21">
+    <row r="190" spans="1:5" ht="21">
       <c r="A190" s="5" t="s">
         <v>171</v>
       </c>
@@ -4324,10 +4437,13 @@
         <v>185</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" ht="21">
+        <v>464</v>
+      </c>
+      <c r="D190" s="10" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" ht="21">
       <c r="A191" s="5" t="s">
         <v>171</v>
       </c>
@@ -4338,7 +4454,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="192" spans="1:3" ht="21">
+    <row r="192" spans="1:5" ht="21">
       <c r="A192" s="5" t="s">
         <v>171</v>
       </c>
@@ -4349,7 +4465,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="21">
+    <row r="193" spans="1:5" ht="21">
       <c r="A193" s="5" t="s">
         <v>171</v>
       </c>
@@ -4360,7 +4476,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="194" spans="1:3" ht="21">
+    <row r="194" spans="1:5" ht="21">
       <c r="A194" s="5" t="s">
         <v>171</v>
       </c>
@@ -4368,10 +4484,13 @@
         <v>189</v>
       </c>
       <c r="C194" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" ht="21">
+        <v>464</v>
+      </c>
+      <c r="D194" s="10" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" ht="21">
       <c r="A195" s="5" t="s">
         <v>171</v>
       </c>
@@ -4379,10 +4498,13 @@
         <v>190</v>
       </c>
       <c r="C195" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" ht="21">
+        <v>464</v>
+      </c>
+      <c r="D195" s="10" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" ht="21">
       <c r="A196" s="5" t="s">
         <v>171</v>
       </c>
@@ -4390,10 +4512,16 @@
         <v>191</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" ht="21">
+        <v>464</v>
+      </c>
+      <c r="D196" s="10" t="s">
+        <v>570</v>
+      </c>
+      <c r="E196" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" ht="21">
       <c r="A197" s="5" t="s">
         <v>171</v>
       </c>
@@ -4404,7 +4532,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="198" spans="1:3" ht="21">
+    <row r="198" spans="1:5" ht="21">
       <c r="A198" s="5" t="s">
         <v>171</v>
       </c>
@@ -4412,10 +4540,16 @@
         <v>193</v>
       </c>
       <c r="C198" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" ht="21">
+        <v>464</v>
+      </c>
+      <c r="D198" s="10" t="s">
+        <v>575</v>
+      </c>
+      <c r="E198" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" ht="21">
       <c r="A199" s="5" t="s">
         <v>171</v>
       </c>
@@ -4426,7 +4560,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="21">
+    <row r="200" spans="1:5" ht="21">
       <c r="A200" s="5" t="s">
         <v>171</v>
       </c>
@@ -4437,7 +4571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="201" spans="1:3" ht="21">
+    <row r="201" spans="1:5" ht="21">
       <c r="A201" s="5" t="s">
         <v>171</v>
       </c>
@@ -4448,7 +4582,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="202" spans="1:3" ht="21">
+    <row r="202" spans="1:5" ht="21">
       <c r="A202" s="5" t="s">
         <v>171</v>
       </c>
@@ -4456,10 +4590,16 @@
         <v>197</v>
       </c>
       <c r="C202" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" ht="21">
+        <v>464</v>
+      </c>
+      <c r="D202" s="10" t="s">
+        <v>574</v>
+      </c>
+      <c r="E202" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" ht="21">
       <c r="A203" s="5" t="s">
         <v>171</v>
       </c>
@@ -4470,7 +4610,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="204" spans="1:3" ht="21">
+    <row r="204" spans="1:5" ht="21">
       <c r="A204" s="5" t="s">
         <v>171</v>
       </c>
@@ -4481,7 +4621,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="205" spans="1:3" ht="21">
+    <row r="205" spans="1:5" ht="21">
       <c r="A205" s="5" t="s">
         <v>171</v>
       </c>
@@ -4492,7 +4632,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="206" spans="1:3" ht="21">
+    <row r="206" spans="1:5" ht="21">
       <c r="A206" s="5" t="s">
         <v>171</v>
       </c>
@@ -4503,7 +4643,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="207" spans="1:3" ht="21">
+    <row r="207" spans="1:5" ht="21">
       <c r="A207" s="5" t="s">
         <v>171</v>
       </c>
@@ -4511,10 +4651,16 @@
         <v>202</v>
       </c>
       <c r="C207" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" ht="21">
+        <v>464</v>
+      </c>
+      <c r="D207" s="10" t="s">
+        <v>569</v>
+      </c>
+      <c r="E207" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" ht="21">
       <c r="A208" s="5" t="s">
         <v>171</v>
       </c>
@@ -4522,7 +4668,10 @@
         <v>203</v>
       </c>
       <c r="C208" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
+      </c>
+      <c r="D208" s="10" t="s">
+        <v>572</v>
       </c>
     </row>
     <row r="209" spans="1:3" ht="21">
@@ -8036,8 +8185,27 @@
     <hyperlink ref="D468" r:id="rId521" xr:uid="{2481017B-FBF7-4C05-862C-0DBDCA6A9D45}"/>
     <hyperlink ref="D173" r:id="rId522" xr:uid="{B2297606-E51B-432B-AA5E-907A9CCEFCE9}"/>
     <hyperlink ref="D172" r:id="rId523" xr:uid="{C6B47040-1FEF-422E-B302-32C42013C191}"/>
+    <hyperlink ref="D110" r:id="rId524" xr:uid="{AF65D8C8-C025-43C2-B0A2-8A1686F5AF23}"/>
+    <hyperlink ref="D111" r:id="rId525" xr:uid="{F434C436-B23C-4D6F-AB45-D4F408E3A18F}"/>
+    <hyperlink ref="D179" r:id="rId526" xr:uid="{A7F5FBB7-650F-4C0D-9290-BCF307F16E17}"/>
+    <hyperlink ref="D178" r:id="rId527" xr:uid="{0A4477F0-8AD1-40AE-92B7-2E1EE7F25B05}"/>
+    <hyperlink ref="D177" r:id="rId528" xr:uid="{0864A854-B368-4965-91B2-BB3C99F478BE}"/>
+    <hyperlink ref="D180" r:id="rId529" xr:uid="{345E4F3C-E9AB-411E-B25F-78FCBEDD4F93}"/>
+    <hyperlink ref="D171" r:id="rId530" xr:uid="{1C9DCCE9-F85C-403B-ADE8-5281E56F6912}"/>
+    <hyperlink ref="D187" r:id="rId531" xr:uid="{892325A6-1532-43A2-9578-C7D0AB5CDD13}"/>
+    <hyperlink ref="D186" r:id="rId532" xr:uid="{43951A73-C13E-4890-A874-C6108EF19F81}"/>
+    <hyperlink ref="D185" r:id="rId533" xr:uid="{02F5C37F-ECF1-4469-B479-BD190C376D10}"/>
+    <hyperlink ref="D188" r:id="rId534" xr:uid="{0C853E68-FD72-4B8E-90BB-6BEE2E024101}"/>
+    <hyperlink ref="D190" r:id="rId535" xr:uid="{26B4908A-4666-4476-9683-F6BB2195DF43}"/>
+    <hyperlink ref="D195" r:id="rId536" xr:uid="{BB26D636-8914-45EA-947C-DB5A8C652CC0}"/>
+    <hyperlink ref="D207" r:id="rId537" xr:uid="{21CC1F4B-319B-411B-B5B5-36812F8E42CD}"/>
+    <hyperlink ref="D196" r:id="rId538" xr:uid="{580A7157-BBAF-4501-A159-0F679CEFF816}"/>
+    <hyperlink ref="D208" r:id="rId539" xr:uid="{F9675502-3B41-4ED3-B80D-7225B1685C9E}"/>
+    <hyperlink ref="D194" r:id="rId540" xr:uid="{CD427CB3-F8D6-4CA7-8AF4-465458E610D5}"/>
+    <hyperlink ref="D202" r:id="rId541" xr:uid="{FC948F3C-CD77-4A83-BD26-5A767170F7CC}"/>
+    <hyperlink ref="D198" r:id="rId542" xr:uid="{E340292F-270F-4C84-A732-793CE7AD58CE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId524"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId543"/>
 </worksheet>
 </file>
</xml_diff>